<commit_message>
Algorithms 101: Fix symbol. Add dict Linked Hash Map for Python 3.7+.
</commit_message>
<xml_diff>
--- a/assets/2015/algorithms-101/Table.xlsx
+++ b/assets/2015/algorithms-101/Table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2840" yWindow="7460" windowWidth="25700" windowHeight="13080" tabRatio="500"/>
+    <workbookView xWindow="5700" yWindow="4040" windowWidth="25700" windowHeight="13080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>std::priority_queue</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -172,10 +172,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>OrderedDict</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>C</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -221,6 +217,14 @@
   </si>
   <si>
     <t>Priority Queue</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dict†, OrderedDict</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>† = Python 3.7+</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -228,12 +232,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
@@ -629,17 +627,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="175" workbookViewId="0">
       <selection activeCell="F18" sqref="A1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
@@ -656,7 +655,7 @@
         <v>16</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1">
@@ -678,7 +677,7 @@
         <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>21</v>
@@ -698,7 +697,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>21</v>
@@ -740,7 +739,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>20</v>
@@ -760,7 +759,7 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -780,7 +779,7 @@
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -799,13 +798,13 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>20</v>
@@ -825,7 +824,7 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -845,10 +844,10 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>21</v>
@@ -859,7 +858,7 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -881,7 +880,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -899,7 +898,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="5:5">
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
       <c r="E18" s="2" t="s">
         <v>13</v>
       </c>
@@ -907,7 +909,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>